<commit_message>
Update required/optional fields in cohort template
- All parent fields marked Optional
- Mandatory changed to Required
- Postcode field marked Required
</commit_message>
<xml_diff>
--- a/app/files/cohort-import-template.xlsx
+++ b/app/files/cohort-import-template.xlsx
@@ -1,17 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_5719E648A8FEFB43BD90EE3E85B327D67D0EC59D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6DB8382-6C52-43C8-863B-F78FE2E808B2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="complete template" sheetId="1" r:id="rId4"/>
+    <sheet name="complete template" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>CHILD_SCHOOL_URN</t>
   </si>
@@ -74,13 +94,13 @@
     <t>PARENT_2_EMAIL</t>
   </si>
   <si>
-    <t xml:space="preserve">Mandatory, 6 digits, numeric, use 888888 for school unknown and 999999 for homeschooled </t>
-  </si>
-  <si>
-    <t>Mandatory: Free text </t>
-  </si>
-  <si>
-    <t>Mandatory: DD/MM/YYYY</t>
+    <t xml:space="preserve">Required, 6 digits, numeric, use 888888 for school unknown and 999999 for homeschooled </t>
+  </si>
+  <si>
+    <t>Required: Free text </t>
+  </si>
+  <si>
+    <t>Required: DD/MM/YYYY</t>
   </si>
   <si>
     <t xml:space="preserve">Optional: Male, Female </t>
@@ -89,13 +109,13 @@
     <t>Optional: Free text </t>
   </si>
   <si>
-    <t>Optional, valid postcode format</t>
+    <t>Required: Valid postcode format</t>
   </si>
   <si>
     <t>Optional: 10 digits, numeric </t>
   </si>
   <si>
-    <t>Must be one of: Mum, Dad, Guardian</t>
+    <t>Optional, must be one of: Mum, Dad, Guardian</t>
   </si>
   <si>
     <t>Optional: Phone number </t>
@@ -104,37 +124,18 @@
     <t>Optional: Email address </t>
   </si>
   <si>
-    <t>Free text </t>
-  </si>
-  <si>
-    <t>Phone number </t>
-  </si>
-  <si>
-    <t>Email address </t>
+    <t>Optional: Free text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
@@ -216,29 +217,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -247,25 +238,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ff0f0f0f"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FF0F0F0F"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -467,7 +518,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -485,7 +536,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -514,7 +565,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -539,7 +590,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -564,7 +615,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -589,7 +640,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -614,7 +665,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -639,7 +690,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -664,7 +715,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -689,7 +740,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -714,7 +765,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -727,9 +778,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -746,7 +803,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -764,7 +821,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -789,7 +846,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -814,7 +871,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -839,7 +896,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -864,7 +921,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -889,7 +946,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -914,7 +971,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -939,7 +996,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -964,7 +1021,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -989,7 +1046,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1002,9 +1059,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1018,7 +1081,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1036,7 +1099,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1065,7 +1128,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1090,7 +1153,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1115,7 +1178,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1140,7 +1203,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1165,7 +1228,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1190,7 +1253,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1215,7 +1278,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1240,7 +1303,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1265,7 +1328,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1278,158 +1341,168 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="32" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.8516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.3516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.1719" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="31.3516" style="1" customWidth="1"/>
-    <col min="13" max="13" width="22.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="21.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="31.1719" style="1" customWidth="1"/>
-    <col min="16" max="16" width="31.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="26.6719" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="31.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="31.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="26.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:18" ht="17.25" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="2">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s" s="2">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="51" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:18" ht="51" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="I2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J2" t="s" s="3">
+      <c r="J2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s" s="3">
+      <c r="K2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s" s="3">
+      <c r="L2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s" s="3">
+      <c r="M2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s" s="3">
+      <c r="N2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s" s="3">
+      <c r="O2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P2" t="s" s="3">
+      <c r="P2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" t="s" s="3">
-        <v>29</v>
-      </c>
-      <c r="R2" t="s" s="3">
-        <v>30</v>
+      <c r="Q2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" ht="16" customHeight="1">
+    <row r="3" spans="1:18" ht="15.95" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1449,7 +1522,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" ht="16" customHeight="1">
+    <row r="4" spans="1:18" ht="15.95" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1469,7 +1542,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" ht="16" customHeight="1">
+    <row r="5" spans="1:18" ht="15.95" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1489,7 +1562,7 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" ht="16" customHeight="1">
+    <row r="6" spans="1:18" ht="15.95" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1509,7 +1582,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
     </row>
-    <row r="7" ht="16" customHeight="1">
+    <row r="7" spans="1:18" ht="15.95" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1529,7 +1602,7 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" ht="16" customHeight="1">
+    <row r="8" spans="1:18" ht="15.95" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1549,7 +1622,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" ht="16" customHeight="1">
+    <row r="9" spans="1:18" ht="15.95" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1569,7 +1642,7 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" ht="16" customHeight="1">
+    <row r="10" spans="1:18" ht="15.95" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1591,7 +1664,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>